<commit_message>
chore: publish IG 1.7.1
</commit_message>
<xml_diff>
--- a/ig/terminology/ValueSet-MedComDiagnosticReportCodesValueset.xlsx
+++ b/ig/terminology/ValueSet-MedComDiagnosticReportCodesValueset.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from MedComDiagnostic" r:id="rId4" sheetId="2"/>
+    <sheet name="Include #0" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.0</t>
+    <t>1.7.1</t>
   </si>
   <si>
     <t>Name</t>

</xml_diff>

<commit_message>
chore: publish IG 1.8.1
</commit_message>
<xml_diff>
--- a/ig/terminology/ValueSet-MedComDiagnosticReportCodesValueset.xlsx
+++ b/ig/terminology/ValueSet-MedComDiagnosticReportCodesValueset.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from MedComDiagnostic" r:id="rId4" sheetId="2"/>
+    <sheet name="Include #0" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.0</t>
+    <t>1.8.1</t>
   </si>
   <si>
     <t>Name</t>

</xml_diff>